<commit_message>
Ajout Watchdog 60 min et release date en parametres
</commit_message>
<xml_diff>
--- a/porte_thingspeaks/Cablage_porte_thingspeaks.xlsx
+++ b/porte_thingspeaks/Cablage_porte_thingspeaks.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="160">
   <si>
     <t>Int</t>
   </si>
@@ -578,6 +578,16 @@
   </si>
   <si>
     <t>!IlsPorte</t>
+  </si>
+  <si>
+    <t>Flash
+On reset</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Low</t>
   </si>
 </sst>
 </file>
@@ -4187,7 +4197,7 @@
   <dimension ref="A1:U41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4207,7 +4217,7 @@
     <col min="13" max="13" width="14" customWidth="1"/>
     <col min="14" max="14" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" customWidth="1"/>
     <col min="17" max="17" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="7" bestFit="1" customWidth="1"/>
@@ -4258,7 +4268,9 @@
       <c r="O1" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="P1" s="21"/>
+      <c r="P1" s="22" t="s">
+        <v>157</v>
+      </c>
       <c r="Q1" s="22"/>
       <c r="R1" s="23"/>
       <c r="S1" s="23"/>
@@ -4285,7 +4297,7 @@
       <c r="M2" s="46"/>
       <c r="N2" s="46"/>
       <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
+      <c r="P2" s="47"/>
       <c r="Q2" s="47"/>
       <c r="R2" s="48"/>
       <c r="S2" s="48"/>
@@ -4312,7 +4324,7 @@
       <c r="M3" s="46"/>
       <c r="N3" s="46"/>
       <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
+      <c r="P3" s="47"/>
       <c r="Q3" s="47"/>
       <c r="R3" s="48"/>
       <c r="S3" s="48"/>
@@ -4339,7 +4351,7 @@
       <c r="M4" s="46"/>
       <c r="N4" s="46"/>
       <c r="O4" s="46"/>
-      <c r="P4" s="46"/>
+      <c r="P4" s="47"/>
       <c r="Q4" s="47"/>
       <c r="R4" s="48"/>
       <c r="S4" s="48"/>
@@ -4366,7 +4378,7 @@
       <c r="M5" s="46"/>
       <c r="N5" s="46"/>
       <c r="O5" s="46"/>
-      <c r="P5" s="46"/>
+      <c r="P5" s="47"/>
       <c r="Q5" s="47"/>
       <c r="R5" s="48"/>
       <c r="S5" s="48"/>
@@ -4399,7 +4411,7 @@
       <c r="M6" s="46"/>
       <c r="N6" s="46"/>
       <c r="O6" s="46"/>
-      <c r="P6" s="46"/>
+      <c r="P6" s="47"/>
       <c r="Q6" s="47"/>
       <c r="R6" s="48"/>
       <c r="S6" s="48"/>
@@ -4434,7 +4446,7 @@
         <v>124</v>
       </c>
       <c r="O7" s="46"/>
-      <c r="P7" s="46"/>
+      <c r="P7" s="47"/>
       <c r="Q7" s="47"/>
       <c r="R7" s="48"/>
       <c r="S7" s="48"/>
@@ -4467,7 +4479,9 @@
       <c r="O8" s="46" t="s">
         <v>149</v>
       </c>
-      <c r="P8" s="46"/>
+      <c r="P8" s="47" t="s">
+        <v>158</v>
+      </c>
       <c r="Q8" s="47"/>
       <c r="R8" s="48"/>
       <c r="S8" s="48"/>
@@ -4498,7 +4512,9 @@
       <c r="M9" s="45"/>
       <c r="N9" s="46"/>
       <c r="O9" s="46"/>
-      <c r="P9" s="46"/>
+      <c r="P9" s="47" t="s">
+        <v>159</v>
+      </c>
       <c r="Q9" s="47"/>
       <c r="R9" s="48"/>
       <c r="S9" s="48"/>

</xml_diff>